<commit_message>
Correccion ajustes de base de datos
se ajusto la coneccion con la base de datos
</commit_message>
<xml_diff>
--- a/Data/Config-QA.xlsx
+++ b/Data/Config-QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saacd\Documentos\UiPath\worldwide medica\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C07B2E-7750-4EED-8794-BED0564EDA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A24E0D1-AAA6-4934-A778-F4744E1A1C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -312,27 +312,15 @@
     <t>jsonCoordenadasUB92</t>
   </si>
   <si>
-    <t>{'datos clientes':{'Pacient Name':['70','165','468','180'],'Billing provider':['45','35','410','67']…</t>
-  </si>
-  <si>
     <t>jsonCoordenadascms1500</t>
   </si>
   <si>
-    <t>{'datos clientes':{'Billing provider':['860','1543','1309','1567'],'Signature':['128','1586','449']…</t>
-  </si>
-  <si>
     <t>jsonCoordenadascms1500V2</t>
   </si>
   <si>
-    <t>{'datos clientes':{'Billing provider':['867','1547','1310','1576'],'Signature':['126','1570','449']…</t>
-  </si>
-  <si>
     <t>jsonCoordenadascms1500V3</t>
   </si>
   <si>
-    <t>{'datos clientes':{'Billing provider':['858','1555','1309','1579'],'Signature':['128','1586','449']…</t>
-  </si>
-  <si>
     <t>credencialCorreo</t>
   </si>
   <si>
@@ -351,9 +339,6 @@
     <t>apiKeyAzure</t>
   </si>
   <si>
-    <t>Produccion/Indemnizaciones/Reclamaciones de salud</t>
-  </si>
-  <si>
     <t>credencialClaimscape</t>
   </si>
   <si>
@@ -394,6 +379,18 @@
   </si>
   <si>
     <t>WWM/Extraccion Formularios/Desarrollo</t>
+  </si>
+  <si>
+    <t>{'datos clientes':{'Pacient Name':['70','165','468','180'],'Billing provider':['45','35','410','67'],'Signature':['410','45','769','68'],'Pacient Account':['800','45','1150','70'],'Federal Tax':['765','110','910','140'],'fecha desde':['900','118','1005','140'],'fecha hasta':['1006','118','1107','140'],'type of bill':['1140','70','1255','100'],'Insured ID':['465','1110','759','1140'],'Diagnosis A':['70','1270','190','1300'],'Diagnosis B':['190','1270','305','1300'],'Diagnosis C':['303','1270','420','1300'],'Diagnosis D':['417','1270','529','1300'],'Cargo Total':['903','970','1045','995']},'cargo1':{'REV CD':['22','454','464','477'],'CPT/HCPCS':['468','454','690','477'],'Fecha':['693','454','796','477'],'Days Or Units':['798','454','916','477'],'cargo':['918','454','1066','477']},'cargo2':{'2REV CD':['22','479','464','502'],'2CPT/HCPCS':['468','479','690','502'],'2Fecha':['693','479','796','502'],'2Days Or Units':['798','479','916','502'],'2cargo':['918','479','1066','502']},'cargo3':{'3REV CD':['22','504','464','525'],'3CPT/HCPCS':['468','504','690','525'],'3Fecha':['693','504','796','525'],'3Days Or Units':['798','504','916','525'],'3cargo':['918','504','1066','525']},'cargo4':{'4REV CD':['22','527','464','552'],'4CPT/HCPCS':['468','527','690','552'],'4Fecha':['693','527','796','552'],'4Days Or Units':['798','527','916','552'],'4cargo':['918','527','1066','552']},'cargo5':{'5REV CD':['22','554','464','577'],'5CPT/HCPCS':['468','554','690','577'],'5Fecha':['693','554','796','577'],'5Days Or Units':['798','554','916','577'],'5cargo':['918','554','1066','577']},'cargo6':{'6REV CD':['22','579','464','602'],'6CPT/HCPCS':['468','579','690','602'],'6Fecha':['693','579','796','602'],'6Days Or Units':['798','579','916','602'],'6cargo':['918','579','1066','602']},'cargo7':{'7REV CD':['22','604','464','627'],'7CPT/HCPCS':['468','604','690','627'],'7Fecha':['693','604','796','627'],'7Days Or Units':['798','604','916','627'],'7cargo':['918','604','1066','627']},'cargo8':{'8REV CD':['22','629','464','652'],'8CPT/HCPCS':['468','629','690','652'],'8Fecha':['693','629','796','652'],'8Days Or Units':['798','629','916','652'],'8cargo':['918','629','1066','652']},'cargo9':{'9REV CD':['22','654','464','677'],'9CPT/HCPCS':['468','654','690','677'],'9Fecha':['693','654','796','677'],'9Days Or Units':['798','654','916','677'],'9cargo':['918','654','1066','677']},'cargo10':{'10REV CD':['22','679','464','700'],'10CPT/HCPCS':['468','679','690','700'],'10Fecha':['693','679','796','700'],'10Days Or Units':['798','679','916','700'],'10cargo':['918','679','1066','700']},'cargo11':{'11REV CD':['22','702','464','727'],'11CPT/HCPCS':['468','702','690','727'],'11Fecha':['693','702','796','727'],'11Days Or Units':['798','702','916','727'],'11cargo':['918','702','1066','727']},'cargo12':{'12REV CD':['22','729','464','754'],'12CPT/HCPCS':['468','729','690','754'],'12Fecha':['693','729','796','754'],'12Days Or Units':['798','729','916','754'],'12cargo':['918','729','1066','754']},'cargo13':{'13REV CD':['22','756','464','779'],'13CPT/HCPCS':['468','756','690','779'],'13Fecha':['693','756','796','779'],'13Days Or Units':['798','756','916','779'],'13cargo':['918','756','1066','779']},'cargo14':{'14REV CD':['22','781','464','800'],'14CPT/HCPCS':['468','781','690','800'],'14Fecha':['693','781','796','800'],'14Days Or Units':['798','781','916','800'],'14cargo':['918','781','1066','800']},'cargo15':{'15REV CD':['22','802','464','828'],'15CPT/HCPCS':['468','802','690','828'],'15Fecha':['693','802','796','828'],'15Days Or Units':['798','802','916','828'],'15cargo':['918','802','1066','828']},'cargo16':{'16REV CD':['22','830','464','850'],'16CPT/HCPCS':['468','830','690','850'],'16Fecha':['693','830','796','850'],'16Days Or Units':['798','830','916','850'],'16cargo':['918','830','1066','850']},'cargo17':{'17REV CD':['22','852','464','878'],'17CPT/HCPCS':['468','852','690','878'],'17Fecha':['693','852','796','878'],'17Days Or Units':['798','852','916','878'],'17cargo':['918','852','1066','878']},'cargo18':{'18REV CD':['22','880','464','900'],'18CPT/HCPCS':['468','880','690','900'],'18Fecha':['693','880','796','900'],'18Days Or Units':['798','880','916','900'],'18cargo':['918','880','1066','900']},'cargo19':{'19REV CD':['22','902','464','925'],'19Fecha':['693','902','796','925'],'19CPT/HCPCS':['468','902','690','925'],'19Days Or Units':['798','902','916','925'],'19cargo':['918','902','1066','925']},'cargo20':{'20REV CD':['22','927','464','950'],'20CPT/HCPCS':['468','927','690','950'],'20Fecha':['693','927','796','950'],'20Days Or Units':['798','927','916','950'],'20cargo':['918','927','1066','950']},'cargo21':{'21REV CD':['22','952','464','978'],'21CPT/HCPCS':['468','952','690','978'],'21Fecha':['693','952','796','978'],'21Days Or Units':['798','952','916','978'],'21cargo':['918','952','1066','978']},'cargo22':{'22REV CD':['22','980','464','1000'],'22CPT/HCPCS':['468','980','690','1000'],'22Fecha':['693','980','796','1000'],'22Days Or Units':['798','980','916','1000'],'22cargo':['918','980','1066','1000']}}</t>
+  </si>
+  <si>
+    <t>{'datos clientes':{'Billing provider':['860','1543','1309','1567'],'Signature':['128','1586','449','1618'],'Cargo Total':['860','1493','1025','1521'],'Pacient Account':['453','1490','671','1523'],'Federal Tax':['126','1490','361','1523'],'Insured ID':['859','293','1050','324'],'Pacient Name':['126','343','553','372'],'Diagnosis A':['158','1045','260','1070'],'Diagnosis B':['352','1045','454','1070'],'Diagnosis C':['550','1045','649','1070'],'Diagnosis D':['743','1055','848','1075']},'cargo1':{'Fecha desde':['130','1200','252','1221'],'Fecha hasta':['260','1200','388','1221'],'Place of service':['390','1200','436','1221'],'CPT/HCPCS':['483','1200','591','1221'],'Modifier1':['594','1200','644','1221'],'Modifier2':['647','1200','689','1221'],'Modifier3':['691','1200','734','1221'],'Modifier4':['736','1200','779','1221'],'Days Or Units':['992','1200','1049','1221'],'cargo':['860','1200','988','1221']},'cargo2':{'2Fecha desde':['130','1245','252','1272'],'2Fecha hasta':['260','1245','388','1272'],'2Place of service':['390','1245','436','1272'],'2CPT/HCPCS':['483','1245','591','1272'],'2Modifier1':['594','1245','644','1272'],'2Modifier2':['647','1245','689','1272'],'2Modifier3':['691','1245','734','1272'],'2Modifier4':['736','1245','779','1272'],'2Days Or Units':['992','1245','1049','1272'],'2cargo':['860','1245','988','1272']},'cargo3':{'3Fecha desde':['130','1294','252','1319'],'3Fecha hasta':['260','1294','388','1319'],'3Place of service':['390','1294','436','1319'],'3CPT/HCPCS':['483','1294','591','1319'],'3Modifier1':['594','1294','644','1319'],'3Modifier2':['647','1294','689','1319'],'3Modifier3':['691','1294','734','1319'],'3Modifier4':['736','1294','779','1319'],'3Days Or Units':['992','1294','1049','1319'],'3cargo':['860','1294','988','1319']},'cargo4':{'4Fecha desde':['130','1346','252','1370'],'4Fecha hasta':['260','1346','388','1370'],'4Place of service':['390','1346','436','1370'],'4CPT/HCPCS':['483','1346','591','1370'],'4Modifier1':['594','1346','644','1370'],'4Modifier2':['647','1346','689','1370'],'4Modifier3':['691','1346','734','1370'],'4Modifier4':['736','1346','779','1370'],'4Days Or Units':['992','1346','1049','1370'],'4cargo':['860','1346','988','1370']},'cargo5':{'5Fecha desde':['130','1396','252','1418'],'5Fecha hasta':['260','1396','388','1418'],'5Place of service':['390','1396','436','1418'],'5CPT/HCPCS':['483','1396','591','1418'],'5Modifier1':['594','1396','644','1418'],'5Modifier2':['647','1396','689','1418'],'5Modifier3':['691','1396','734','1418'],'5Modifier4':['736','1396','779','1418'],'5Days Or Units':['992','1396','1049','1418'],'5cargo':['860','1396','988','1418']},'cargo6':{'6Fecha desde':['130','1445','252','1469'],'6Fecha hasta':['260','1445','388','1469'],'6Place of service':['390','1445','436','1469'],'6CPT/HCPCS':['483','1445','591','1469'],'6Modifier1':['594','1445','644','1469'],'6Modifier2':['647','1445','689','1469'],'6Modifier3':['691','1445','734','1469'],'6Modifier4':['736','1445','779','1469'],'6Days Or Units':['991','1445','1048','1469'],'6cargo':['860','1445','988','1469']}}</t>
+  </si>
+  <si>
+    <t>{'datos clientes':{'Billing provider':['867','1547','1310','1576'],'Signature':['126','1570','449','1610'],'Pacient Account':['450','1490','696','1526'],'Federal Tax':['126','1491','350','1525'],'Pacient Name':['126','334','550','370'],'Insured ID':['850','289','1050','314'],'Diagnosis A':['158','1050','302','1066'],'Diagnosis B':['340','1050','484','1066'],'Diagnosis C':['520','1050','664','1066'],'Diagnosis D':['702','1050','844','1066'],'Cargo Total':['951','1501','1022','1515']},'cargo1':{'Fecha desde':['125','1215','252','1239'],'Fecha hasta':['258','1215','388','1239'],'Place of service':['393','1215','438','1239'],'CPT/HCPCS':['490','1215','594','1239'],'Modifier1':['599','1215','648','1239'],'Modifier2':['652','1215','691','1239'],'Modifier3':['697','1215','736','1239'],'Modifier4':['743','1215','785','1239'],'Days Or Units':['999','1215','1056','1239'],'cargo':['867','1215','994','1239']},'cargo2':{'2Fecha desde':['125','1264','252','1285'],'2Fecha hasta':['258','1264','388','1285'],'2Place of service':['393','1264','438','1285'],'2CPT/HCPCS':['490','1264','594','1285'],'2Modifier1':['599','1264','648','1285'],'2Modifier2':['652','1264','691','1285'],'2Modifier3':['697','1264','736','1285'],'2Modifier4':['743','1264','785','1285'],'2Days Or Units':['999','1264','1056','1285'],'2cargo':['867','1264','994','1285']},'cargo3':{'3Fecha desde':['125','1311','252','1333'],'3Fecha hasta':['258','1311','388','1333'],'3Place of service':['393','1311','438','1333'],'3CPT/HCPCS':['490','1311','594','1333'],'3Modifier1':['599','1311','648','1333'],'3Modifier2':['652','1311','691','1333'],'3Modifier3':['697','1311','736','1333'],'3Modifier4':['743','1311','785','1333'],'3Days Or Units':['999','1311','1056','1333'],'3cargo':['867','1311','994','1333']},'cargo4':{'4Fecha desde':['125','1358','252','1381'],'4Fecha hasta':['258','1358','388','1381'],'4Place of service':['393','1358','438','1381'],'4CPT/HCPCS':['490','1358','594','1381'],'4Modifier1':['599','1358','648','1381'],'4Modifier2':['652','1358','691','1381'],'4Modifier3':['697','1358','736','1381'],'4Modifier4':['743','1358','785','1381'],'4Days Or Units':['999','1358','1056','1381'],'4cargo':['867','1358','994','1381']},'cargo5':{'5Fecha desde':['125','1406','252','1429'],'5Fecha hasta':['258','1406','388','1429'],'5Place of service':['393','1406','438','1429'],'5CPT/HCPCS':['490','1406','594','1429'],'5Modifier1':['599','1406','648','1429'],'5Modifier2':['652','1406','691','1429'],'5Modifier3':['697','1406','736','1429'],'5Modifier4':['743','1406','785','1429'],'5Days Or Units':['999','1406','1056','1429'],'5cargo':['867','1406','994','1429']},'cargo6':{'6Fecha desde':['125','1453','252','1476'],'6Fecha hasta':['258','1453','388','1476'],'6Place of service':['393','1453','438','1476'],'6CPT/HCPCS':['490','1453','594','1476'],'6Modifier1':['599','1453','648','1476'],'6Modifier2':['652','1453','691','1476'],'6Modifier3':['697','1453','736','1476'],'6Modifier4':['743','1453','785','1476'],'6Days Or Units':['999','1453','1056','1476'],'6cargo':['867','1453','994','1476']}}</t>
+  </si>
+  <si>
+    <t>{'datos clientes':{'Billing provider':['858','1555','1309','1579'],'Signature':['128','1586','449','1618'],'Pacient Account':['453','1503','671','1525'],'Federal Tax':['126','1500','361','1525'],'Pacient Name':['126','343','553','372'],'Insured ID':['859','293','1050','324'],'Diagnosis A':['158','1045','260','1070'],'Diagnosis B':['352','1045','454','1070'],'Diagnosis C':['550','1045','649','1070'],'Diagnosis D':['743','1055','848','1075'],'Cargo Total':['858','1500','1025','1525']},'cargo1':{'Fecha desde':['128','1200','252','1221'],'Fecha hasta':['260','1200','388','1221'],'Place of service':['392','1200','434','1221'],'CPT/HCPCS':['483','1200','586','1221'],'Modifier1':['590','1200','644','1221'],'Modifier2':['647','1200','689','1221'],'Modifier3':['691','1200','734','1221'],'Modifier4':['736','1200','779','1221'],'Days Or Units':['995','1200','1052','1221'],'cargo':['858','1200','990','1221']},'cargo2':{'2Fecha desde':['128','1245','252','1271'],'2Fecha hasta':['260','1245','388','1271'],'2Place of service':['392','1245','434','1271'],'2CPT/HCPCS':['483','1245','586','1271'],'2Modifier1':['590','1245','644','1271'],'2Modifier2':['647','1245','689','1271'],'2Modifier3':['691','1245','734','1271'],'2Modifier4':['736','1245','779','1271'],'2Days Or Units':['995','1245','1052','1271'],'2cargo':['858','1245','990','1271']},'cargo3':{'3Fecha desde':['128','1298','252','1321'],'3Fecha hasta':['260','1298','388','1321'],'3Place of service':['392','1298','434','1321'],'3CPT/HCPCS':['483','1298','586','1321'],'3Modifier1':['590','1298','644','1321'],'3Modifier2':['647','1298','689','1321'],'3Modifier3':['691','1298','734','1321'],'3Modifier4':['736','1298','779','1321'],'3Days Or Units':['995','1298','1052','1321'],'3cargo':['858','1298','990','1321']},'cargo4':{'4Fecha desde':['128','1348','252','1372'],'4Fecha hasta':['260','1348','388','1372'],'4Place of service':['392','1348','434','1372'],'4CPT/HCPCS':['483','1348','586','1372'],'4Modifier1':['590','1348','644','1372'],'4Modifier2':['647','1348','689','1372'],'4Modifier3':['691','1348','734','1372'],'4Modifier4':['736','1348','779','1372'],'4Days Or Units':['995','1348','1052','1372'],'4cargo':['858','1348','990','1372']},'cargo5':{'5Fecha desde':['128','1400','252','1422'],'5Fecha hasta':['260','1400','388','1422'],'5Place of service':['392','1400','434','1422'],'5CPT/HCPCS':['483','1400','586','1422'],'5Modifier1':['590','1400','644','1422'],'5Modifier2':['647','1400','689','1422'],'5Modifier3':['691','1400','734','1422'],'5Modifier4':['736','1400','779','1422'],'5Days Or Units':['995','1400','1052','1422'],'5cargo':['858','1400','990','1422']},'cargo6':{'6Fecha desde':['128','1449','252','1472'],'6Fecha hasta':['260','1449','388','1472'],'6Place of service':['392','1449','434','1472'],'6CPT/HCPCS':['483','1449','586','1472'],'6Modifier1':['590','1449','644','1472'],'6Modifier2':['647','1449','689','1472'],'6Modifier3':['691','1449','734','1472'],'6Modifier4':['736','1449','779','1472'],'6Days Or Units':['991','1449','1048','1472'],'6cargo':['858','1449','990','1472']}}</t>
   </si>
 </sst>
 </file>
@@ -457,7 +454,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +464,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,6 +514,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -828,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="27" customHeight="1"/>
@@ -1132,32 +1137,32 @@
       <c r="A34" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>96</v>
+      <c r="B34" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="27" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="27" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="27" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="27" customHeight="1">
@@ -1202,23 +1207,23 @@
     </row>
     <row r="43" spans="1:2" ht="27" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="27" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="27" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B45" s="4">
         <v>587</v>
@@ -1226,10 +1231,10 @@
     </row>
     <row r="46" spans="1:2" ht="27" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="27" customHeight="1">
@@ -1237,15 +1242,15 @@
         <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="27" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="27" customHeight="1">
@@ -1330,10 +1335,10 @@
     </row>
     <row r="59" spans="1:2" ht="27" customHeight="1">
       <c r="A59" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="27" customHeight="1">
@@ -1346,10 +1351,10 @@
     </row>
     <row r="61" spans="1:2" ht="27" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="27" customHeight="1">
@@ -1402,34 +1407,34 @@
     </row>
     <row r="68" spans="1:2" ht="27" customHeight="1">
       <c r="A68" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="27" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="27" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="27" customHeight="1">
       <c r="A71" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>